<commit_message>
feat(xlsx-import): support arbitrary status
</commit_message>
<xml_diff>
--- a/CGTeamWork返修样表.xlsx
+++ b/CGTeamWork返修样表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13005"/>
+    <workbookView windowWidth="21000" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>镜头</t>
   </si>
@@ -42,7 +42,7 @@
     <t>客户</t>
   </si>
   <si>
-    <t>返修</t>
+    <t>Approve</t>
   </si>
   <si>
     <t>test</t>
@@ -58,7 +58,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,13 +97,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -227,30 +220,174 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -263,151 +400,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,148 +516,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1023,7 +1016,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="4"/>

</xml_diff>